<commit_message>
Updated diary as of 21 Jan 2020
This had better work, command-line git drives me nuts. I want to automate the whole process, or at least most of it, and git doesn't behave as expected (i.e. git pull does not actually pull).
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -124,7 +124,73 @@
     <t xml:space="preserve">Craving some Mexican food</t>
   </si>
   <si>
-    <t xml:space="preserve">Etc.</t>
+    <t xml:space="preserve">15 Jan 2020 (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2100-2300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research various projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Found a few projects like ghidra, micrometer, etc…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Jan 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Jan 2020 (Sa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2145-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harry, Deon, Thuc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discuss findings and decide on project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After debating for a while, we decided to go with a project called Runelite, which is a client for the popular game RuneScape.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The usual quirks of group decisions come up – the paradox of choice forces a lengthy debate on where to proceed, especially since metering a project’s appeal comes from the group members’ passions for each project. No two members have the same exact passions, not at least in this group, so the decision is difficulit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feeling good after dancing out (some of) the stress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Jan 2020 (Su)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure out a clean method to synchronize 265’s, my, and my computer’s local W2020 repositories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if you see this message in the 265P repository then what I did works.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Jan 2020 (Tu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1200-1250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read and annotate Jonas Juselius’s “Git in a Nutshell” document to understand Git and possibly automate updating the diary and project files and such; the GitHub web interface can help only so much. The internet is not much help either; the GitHub documentation isn’t very clear.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I read and annotated the whole document and can reference it when I need it. It is a lot to remember and I need time to get used to git.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I printed this document long ago and never went through it completely because I never had to use git or GitHub. Git overwhelms and has many features that I will discover in time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I should eat lunch before heading off to campus.</t>
   </si>
 </sst>
 </file>
@@ -424,10 +490,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -634,58 +700,112 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+    <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
+    <row r="18" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="7"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
@@ -694,7 +814,7 @@
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
@@ -721,7 +841,7 @@
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
@@ -1652,6 +1772,15 @@
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
       <c r="G126" s="9"/>
+    </row>
+    <row r="127" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated diary as of 28 Jan 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -191,6 +191,42 @@
   </si>
   <si>
     <t xml:space="preserve">I should eat lunch before heading off to campus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Jan 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about UML and mental models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a pattern to the way people analyze code. Sometimes it’s brute force as I often do, by printing and reading source code on paper. Sometimes I can search smartly using IntelliJ, grep, or find. The key idea is that as with any programming system, it’s more efficient to think smartly first to narrow the search space (although it doesn’t feel efficient). Then when you run out of options you either brute force the system or move on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rather tired; three-hour lectures in a sealed room in the evening are not easy to bear. At least Andre lets us practice our skills and get up and move around.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 Jan 2020 (Tu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1415-1445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture 3 homework: UML diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We already discussed some logistics during the weekend (and the Lunar festivities threw us off). Deon set up the UML diagram and looks to print it out for us to stitch together.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhausted. Not from the coursework from this quarter, but from the last 16-17 months of craziness.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1500-1530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaj’s Git mini lecture</t>
   </si>
 </sst>
 </file>
@@ -200,7 +236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -222,6 +258,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -247,6 +290,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
@@ -286,14 +336,6 @@
     <font>
       <i val="true"/>
       <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -359,13 +401,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -374,32 +416,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -407,7 +441,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -492,103 +534,103 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="34.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="1" width="34.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -611,7 +653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
@@ -628,11 +670,11 @@
         <v>18</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -650,7 +692,7 @@
         <v>First lecture, meet Andre</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -673,7 +715,7 @@
       <c r="F12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -696,7 +738,7 @@
         <v>Learn the basics of git and GitHub, GitHub’s [hello world] example</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -717,7 +759,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
@@ -734,7 +776,7 @@
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
@@ -755,7 +797,7 @@
       <c r="F16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -776,7 +818,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
@@ -797,990 +839,1024 @@
       <c r="F18" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
+    <row r="19" customFormat="false" ht="156.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
+      <c r="G20" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="31" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="9"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="9"/>
-    </row>
-    <row r="34" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="9"/>
-    </row>
-    <row r="36" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
-      <c r="G36" s="9"/>
-    </row>
-    <row r="37" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
-      <c r="G37" s="9"/>
-    </row>
-    <row r="38" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
-      <c r="G39" s="9"/>
-    </row>
-    <row r="40" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="9"/>
-    </row>
-    <row r="41" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
-      <c r="G41" s="9"/>
-    </row>
-    <row r="42" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="9"/>
-    </row>
-    <row r="43" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="9"/>
-    </row>
-    <row r="44" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
-      <c r="G44" s="9"/>
-    </row>
-    <row r="45" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="9"/>
-    </row>
-    <row r="46" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="47" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
-      <c r="G47" s="9"/>
-    </row>
-    <row r="48" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="49" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
-      <c r="G49" s="9"/>
-    </row>
-    <row r="50" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
-      <c r="G50" s="9"/>
-    </row>
-    <row r="51" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
-      <c r="G51" s="9"/>
-    </row>
-    <row r="52" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
-      <c r="G52" s="9"/>
-    </row>
-    <row r="53" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
-      <c r="G53" s="9"/>
-    </row>
-    <row r="54" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
-      <c r="G54" s="9"/>
-    </row>
-    <row r="55" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
-      <c r="G55" s="9"/>
-    </row>
-    <row r="56" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
-      <c r="G56" s="9"/>
-    </row>
-    <row r="57" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G56" s="8"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
-      <c r="G57" s="9"/>
-    </row>
-    <row r="58" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
-      <c r="G58" s="9"/>
-    </row>
-    <row r="59" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
-      <c r="G59" s="9"/>
-    </row>
-    <row r="60" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G59" s="8"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
-      <c r="G60" s="9"/>
-    </row>
-    <row r="61" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G60" s="8"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="9"/>
-    </row>
-    <row r="62" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
-      <c r="G62" s="9"/>
-    </row>
-    <row r="63" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G62" s="8"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
-      <c r="G63" s="9"/>
-    </row>
-    <row r="64" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
-      <c r="G64" s="9"/>
-    </row>
-    <row r="65" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G64" s="8"/>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
-      <c r="G65" s="9"/>
-    </row>
-    <row r="66" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G65" s="8"/>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
-      <c r="G66" s="9"/>
-    </row>
-    <row r="67" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G66" s="8"/>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
-      <c r="G67" s="9"/>
-    </row>
-    <row r="68" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G67" s="8"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
-      <c r="G68" s="9"/>
-    </row>
-    <row r="69" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G68" s="8"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
-      <c r="G69" s="9"/>
-    </row>
-    <row r="70" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G69" s="8"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
-      <c r="G71" s="9"/>
-    </row>
-    <row r="72" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
-      <c r="G72" s="9"/>
-    </row>
-    <row r="73" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
-      <c r="G73" s="9"/>
-    </row>
-    <row r="74" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G73" s="8"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
-      <c r="G74" s="9"/>
-    </row>
-    <row r="75" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G74" s="8"/>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
-      <c r="G75" s="9"/>
-    </row>
-    <row r="76" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G75" s="8"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
-      <c r="G76" s="9"/>
-    </row>
-    <row r="77" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G76" s="8"/>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
-      <c r="G77" s="9"/>
-    </row>
-    <row r="78" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G77" s="8"/>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
-      <c r="G78" s="9"/>
-    </row>
-    <row r="79" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G78" s="8"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
       <c r="F79" s="8"/>
-      <c r="G79" s="9"/>
-    </row>
-    <row r="80" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G79" s="8"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
-      <c r="G80" s="9"/>
-    </row>
-    <row r="81" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G80" s="8"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8"/>
       <c r="F81" s="8"/>
-      <c r="G81" s="9"/>
-    </row>
-    <row r="82" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G81" s="8"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
-      <c r="G82" s="9"/>
-    </row>
-    <row r="83" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G82" s="8"/>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
-      <c r="G83" s="9"/>
-    </row>
-    <row r="84" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G83" s="8"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
-      <c r="G84" s="9"/>
-    </row>
-    <row r="85" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G84" s="8"/>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
       <c r="F85" s="8"/>
-      <c r="G85" s="9"/>
-    </row>
-    <row r="86" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G85" s="8"/>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
       <c r="F86" s="8"/>
-      <c r="G86" s="9"/>
-    </row>
-    <row r="87" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G86" s="8"/>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
       <c r="F87" s="8"/>
-      <c r="G87" s="9"/>
-    </row>
-    <row r="88" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G87" s="8"/>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
       <c r="F88" s="8"/>
-      <c r="G88" s="9"/>
-    </row>
-    <row r="89" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G88" s="8"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="8"/>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
-      <c r="G89" s="9"/>
-    </row>
-    <row r="90" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G89" s="8"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="8"/>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
       <c r="E90" s="8"/>
       <c r="F90" s="8"/>
-      <c r="G90" s="9"/>
-    </row>
-    <row r="91" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G90" s="8"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
       <c r="F91" s="8"/>
-      <c r="G91" s="9"/>
-    </row>
-    <row r="92" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G91" s="8"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="8"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
       <c r="F92" s="8"/>
-      <c r="G92" s="9"/>
-    </row>
-    <row r="93" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G92" s="8"/>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
       <c r="F93" s="8"/>
-      <c r="G93" s="9"/>
-    </row>
-    <row r="94" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G93" s="8"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
       <c r="E94" s="8"/>
       <c r="F94" s="8"/>
-      <c r="G94" s="9"/>
-    </row>
-    <row r="95" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G94" s="8"/>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
       <c r="E95" s="8"/>
       <c r="F95" s="8"/>
-      <c r="G95" s="9"/>
-    </row>
-    <row r="96" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G95" s="8"/>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
       <c r="F96" s="8"/>
-      <c r="G96" s="9"/>
-    </row>
-    <row r="97" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G96" s="8"/>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
       <c r="F97" s="8"/>
-      <c r="G97" s="9"/>
-    </row>
-    <row r="98" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G97" s="8"/>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
       <c r="E98" s="8"/>
       <c r="F98" s="8"/>
-      <c r="G98" s="9"/>
-    </row>
-    <row r="99" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G98" s="8"/>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
       <c r="E99" s="8"/>
       <c r="F99" s="8"/>
-      <c r="G99" s="9"/>
-    </row>
-    <row r="100" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G99" s="8"/>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
       <c r="E100" s="8"/>
       <c r="F100" s="8"/>
-      <c r="G100" s="9"/>
-    </row>
-    <row r="101" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G100" s="8"/>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="8"/>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
       <c r="E101" s="8"/>
       <c r="F101" s="8"/>
-      <c r="G101" s="9"/>
-    </row>
-    <row r="102" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G101" s="8"/>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
       <c r="E102" s="8"/>
       <c r="F102" s="8"/>
-      <c r="G102" s="9"/>
-    </row>
-    <row r="103" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G102" s="8"/>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
       <c r="E103" s="8"/>
       <c r="F103" s="8"/>
-      <c r="G103" s="9"/>
-    </row>
-    <row r="104" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G103" s="8"/>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
       <c r="E104" s="8"/>
       <c r="F104" s="8"/>
-      <c r="G104" s="9"/>
-    </row>
-    <row r="105" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G104" s="8"/>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
       <c r="F105" s="8"/>
-      <c r="G105" s="9"/>
-    </row>
-    <row r="106" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G105" s="8"/>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="8"/>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
       <c r="E106" s="8"/>
       <c r="F106" s="8"/>
-      <c r="G106" s="9"/>
-    </row>
-    <row r="107" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G106" s="8"/>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8"/>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
       <c r="E107" s="8"/>
       <c r="F107" s="8"/>
-      <c r="G107" s="9"/>
-    </row>
-    <row r="108" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G107" s="8"/>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
-      <c r="G108" s="9"/>
-    </row>
-    <row r="109" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G108" s="8"/>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
       <c r="E109" s="8"/>
       <c r="F109" s="8"/>
-      <c r="G109" s="9"/>
-    </row>
-    <row r="110" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G109" s="8"/>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
       <c r="E110" s="8"/>
       <c r="F110" s="8"/>
-      <c r="G110" s="9"/>
-    </row>
-    <row r="111" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G110" s="8"/>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
-      <c r="G111" s="9"/>
-    </row>
-    <row r="112" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G111" s="8"/>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="8"/>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
       <c r="E112" s="8"/>
       <c r="F112" s="8"/>
-      <c r="G112" s="9"/>
-    </row>
-    <row r="113" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G112" s="8"/>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
       <c r="E113" s="8"/>
       <c r="F113" s="8"/>
-      <c r="G113" s="9"/>
-    </row>
-    <row r="114" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G113" s="8"/>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="8"/>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
       <c r="E114" s="8"/>
       <c r="F114" s="8"/>
-      <c r="G114" s="9"/>
-    </row>
-    <row r="115" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G114" s="8"/>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="8"/>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
       <c r="E115" s="8"/>
       <c r="F115" s="8"/>
-      <c r="G115" s="9"/>
-    </row>
-    <row r="116" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G115" s="8"/>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
-      <c r="G116" s="9"/>
-    </row>
-    <row r="117" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G116" s="8"/>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="8"/>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
-      <c r="G117" s="9"/>
-    </row>
-    <row r="118" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G117" s="8"/>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
-      <c r="G118" s="9"/>
-    </row>
-    <row r="119" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G118" s="8"/>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="8"/>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
-      <c r="G119" s="9"/>
-    </row>
-    <row r="120" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G119" s="8"/>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="8"/>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
-      <c r="G120" s="9"/>
-    </row>
-    <row r="121" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G120" s="8"/>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="8"/>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
       <c r="E121" s="8"/>
       <c r="F121" s="8"/>
-      <c r="G121" s="9"/>
-    </row>
-    <row r="122" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G121" s="8"/>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
-      <c r="G122" s="9"/>
-    </row>
-    <row r="123" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G122" s="8"/>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="8"/>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
-      <c r="G123" s="9"/>
-    </row>
-    <row r="124" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G123" s="8"/>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
       <c r="E124" s="8"/>
       <c r="F124" s="8"/>
-      <c r="G124" s="9"/>
-    </row>
-    <row r="125" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G124" s="8"/>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="8"/>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
-      <c r="G125" s="9"/>
-    </row>
-    <row r="126" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G125" s="8"/>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="8"/>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
-      <c r="G126" s="9"/>
-    </row>
-    <row r="127" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G126" s="8"/>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="8"/>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
       <c r="E127" s="8"/>
       <c r="F127" s="8"/>
-      <c r="G127" s="9"/>
+      <c r="G127" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated diary as of 29 Jan 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -223,10 +223,28 @@
     <t xml:space="preserve">Exhausted. Not from the coursework from this quarter, but from the last 16-17 months of craziness.</t>
   </si>
   <si>
-    <t xml:space="preserve">1500-1530</t>
+    <t xml:space="preserve">1500-1600</t>
   </si>
   <si>
     <t xml:space="preserve">Kaj’s Git mini lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Jan 2020 (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1430-1515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Runelite up and running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It works. IT WORKS! It nor I can do anything meaningful because I know little about Runescape.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This project also introduces me to Maven and Runescape. What boggles me is how a project has multiple build tools like Gradle, Maven, and more.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full. Just downed four fish tacos and am waiting for teammates to come into the lab.</t>
   </si>
 </sst>
 </file>
@@ -534,8 +552,8 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -904,14 +922,28 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+    <row r="22" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>

</xml_diff>

<commit_message>
Updated diary as of 30 Jan 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -245,6 +245,51 @@
   </si>
   <si>
     <t xml:space="preserve">Full. Just downed four fish tacos and am waiting for teammates to come into the lab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1540-1710</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on third lecture’s homework and write up the component findings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deon printed the UML diagram and taped everything together. It’s as messy as we expected. We chose which components to highlight. We wrote up on where the components fit in the UML diagram.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I came in 30 minutes early. Teammates came 40 minutes late. People are busy and traffic is not nice. The difference in time gives a few moments to breathe and observe the lab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1910-1945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We continued discussing the diagram and what components to select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We chose Metronome* and ScreenMarkers and found Metronome* on the diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2300-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalized the writeup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Jan 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More tired than usual. Nutrition and exercise aren’t the issue; something else is wrong.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1135-1220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look at the homework once more. Will look at UML diagram later today to make sure everything is correct.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Things look good to go.</t>
   </si>
 </sst>
 </file>
@@ -552,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -945,48 +990,104 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+    <row r="23" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="A25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+    <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f aca="false">D25</f>
+        <v>Finalized the writeup</v>
+      </c>
+      <c r="E26" s="8" t="str">
+        <f aca="false">E25</f>
+        <v>Finalized the writeup</v>
+      </c>
       <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="G26" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>

</xml_diff>

<commit_message>
Updated diary as of 30 Jan 2020, at 1635
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -290,6 +290,15 @@
   </si>
   <si>
     <t xml:space="preserve">Things look good to go.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1545-1700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalize writeup, finalize UML diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mission accomplished</t>
   </si>
 </sst>
 </file>
@@ -598,7 +607,7 @@
   <dimension ref="A1:G127"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1091,12 +1100,22 @@
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+    <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>

</xml_diff>

<commit_message>
Updated diary as of 6 Feb 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -299,6 +299,36 @@
   </si>
   <si>
     <t xml:space="preserve">Mission accomplished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Jan 2020 (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1710-2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on fourth lecture’s homework while simutaneously paying attention to the 261 lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We finished documenting the first feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decisions, decisions! It’s hard to make a choice of features when there are so many! Also in Runeline a large chunk of the code is plugins. So the hunt for essential features became a lot harder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because the classes are in sequence, I have to work on the assignments in sequence. So the work for this class will always be at the tail end of the weekly schedule.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We finished documenting the second feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Jan 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0030</t>
   </si>
 </sst>
 </file>
@@ -606,8 +636,8 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1119,30 +1149,68 @@
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+    <row r="29" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="8" t="str">
+        <f aca="false">C29</f>
+        <v>Harry, Deon, Thuc</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f aca="false">D29</f>
+        <v>Work on fourth lecture’s homework while simutaneously paying attention to the 261 lecture</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+    <row r="31" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f aca="false">D30</f>
+        <v>Work on fourth lecture’s homework while simutaneously paying attention to the 261 lecture</v>
+      </c>
+      <c r="E31" s="8" t="str">
+        <f aca="false">E30</f>
+        <v>We finished documenting the second feature</v>
+      </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>

</xml_diff>

<commit_message>
Updated diary as of 6 Feb 2020 (#261)
* Updated diary as of 30 Jan 2020, at 1635

* Updated diary as of 6 Feb 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -290,6 +290,45 @@
   </si>
   <si>
     <t xml:space="preserve">Things look good to go.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1545-1700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalize writeup, finalize UML diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mission accomplished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Jan 2020 (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1710-2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on fourth lecture’s homework while simutaneously paying attention to the 261 lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We finished documenting the first feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decisions, decisions! It’s hard to make a choice of features when there are so many! Also in Runeline a large chunk of the code is plugins. So the hunt for essential features became a lot harder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because the classes are in sequence, I have to work on the assignments in sequence. So the work for this class will always be at the tail end of the weekly schedule.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We finished documenting the second feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Jan 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0030</t>
   </si>
 </sst>
 </file>
@@ -597,8 +636,8 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1091,39 +1130,87 @@
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+    <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+    <row r="29" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="8" t="str">
+        <f aca="false">C29</f>
+        <v>Harry, Deon, Thuc</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f aca="false">D29</f>
+        <v>Work on fourth lecture’s homework while simutaneously paying attention to the 261 lecture</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+    <row r="31" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f aca="false">D30</f>
+        <v>Work on fourth lecture’s homework while simutaneously paying attention to the 261 lecture</v>
+      </c>
+      <c r="E31" s="8" t="str">
+        <f aca="false">E30</f>
+        <v>We finished documenting the second feature</v>
+      </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>

</xml_diff>

<commit_message>
Updated diary as of 13 Feb 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -344,6 +344,39 @@
   </si>
   <si>
     <t xml:space="preserve">I need some fruits and vegetables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Jan 2020 (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2245-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study for tomorrow’s midterm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got through the lectures and online articles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don’t procrastinate out of laziness; the past week or so were full of chaos, both in and out of academia. On the bright side, the lecture recordings help tremendously with the studying.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feeling fine, just need a smoothie. I’ll get one on the way to class tomorrow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 Jan 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study for today’s midterm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as yesterday. Will finish studying later today.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stomach is active, just need a smoothie. I’ll get one on the way to class today.</t>
   </si>
 </sst>
 </file>
@@ -652,7 +685,7 @@
   <dimension ref="A1:G127"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1250,23 +1283,52 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
+    <row r="33" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="8" t="str">
+        <f aca="false">F33</f>
+        <v>I don’t procrastinate out of laziness; the past week or so were full of chaos, both in and out of academia. On the bright side, the lecture recordings help tremendously with the studying.</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>

</xml_diff>

<commit_message>
Updated diary as of 20 Feb 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="133">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -386,6 +386,61 @@
   </si>
   <si>
     <t xml:space="preserve">I decided not to drink the whole smoothie. Even though it’s advertised as no added sugar, I don’t believe so.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Feb 2020 (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2200-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supertask by working on latest homework, harassment training, and 264 lab at the same time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished all, just need to review homework for this class with teammates tomorrow in lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Feb 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished all, just need to review homework for this class with teammates today in lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1615-1640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look at homework one last time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submitted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We spent more time deciding whether the document was good enough than actually working on it.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <strike val="true"/>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Need food and water. Badly.</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Went to lunch while waiting for Deon and Thuc to arrive.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -395,7 +450,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -500,6 +555,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i val="true"/>
+      <strike val="true"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -570,7 +634,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -609,6 +673,10 @@
     </xf>
     <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -693,14 +761,14 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="1" width="34.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1361,32 +1429,67 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+    <row r="36" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+    <row r="37" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="8" t="str">
+        <f aca="false">D36</f>
+        <v>Supertask by working on latest homework, harassment training, and 264 lab at the same time</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
+    <row r="38" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>

</xml_diff>

<commit_message>
Updated diary as of 24 Feb 2020. If this branch shows any extra commits other than the latest diary update, ignore them. Those are the brainchildren of me fiddling around with git.
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="137">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -441,6 +441,18 @@
       </rPr>
       <t xml:space="preserve"> Went to lunch while waiting for Deon and Thuc to arrive.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Feb 2020 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1247-1300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix GitHub pull requests at Kaj’s request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I hope GitHub doesn’t merge pull requests again. Team pay4grade aren’t on good terms with Kaj at the moment, so anything that fuses the situation among us doesn’t help.</t>
   </si>
 </sst>
 </file>
@@ -761,14 +773,14 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B33" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="1" width="34.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1491,13 +1503,25 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
+    <row r="39" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="G39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated diary as of 24 Feb 2020. (#392)
* Added homework3 as separate pull request

* Updated diary as of 24 Feb 2020. If this branch shows any extra commits other than the latest diary update, ignore them. Those are the brainchildren of me fiddling around with git.
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="137">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -441,6 +441,18 @@
       </rPr>
       <t xml:space="preserve"> Went to lunch while waiting for Deon and Thuc to arrive.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Feb 2020 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1247-1300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix GitHub pull requests at Kaj’s request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I hope GitHub doesn’t merge pull requests again. Team pay4grade aren’t on good terms with Kaj at the moment, so anything that fuses the situation among us doesn’t help.</t>
   </si>
 </sst>
 </file>
@@ -761,14 +773,14 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B33" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="1" width="34.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1491,13 +1503,25 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
+    <row r="39" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="G39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated diary as of 27 Feb 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="155">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -453,6 +453,82 @@
   </si>
   <si>
     <t xml:space="preserve">I hope GitHub doesn’t merge pull requests again. Team pay4grade aren’t on good terms with Kaj at the moment, so anything that fuses the situation among us doesn’t help.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I forget what day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1700-I don’t remember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on assignments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deon systematically figured out RuneLite’s architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Today I have a monster diet. Android programming (from other courses) takes a lot of energy when doing for the first time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 Feb 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0100-0200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We glossed over the document as the chaos from 261 kept us largely busy today</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding the architecture of a system is not easy, especially when people’s interpretations differ. Software is intangible and there is no realistic way (at least, of my knowledge) to verify whether nontrivial software can match their corresponding architecture.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhausted, once again, from the chaos of 261.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1435-1525</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Look at homework </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <strike val="true"/>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">one last time.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting for rest of team to show up. It’s 1600 and the others aren’t here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full. Just downed a whole Blaze Pizza (honestly, they’re not that big to begin with). My body is full of tomatoes now. Also, Sibelius’s Finlandia keeps my mood up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 Feb 20020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1620-1640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalize the homework.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pull request sent in.</t>
   </si>
 </sst>
 </file>
@@ -773,8 +849,8 @@
   </sheetPr>
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B33" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1524,39 +1600,87 @@
       </c>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+    <row r="40" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="G40" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
+      <c r="G42" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="A43" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
     </row>

</xml_diff>

<commit_message>
Updated diary as of 5 Mar 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="169">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -553,6 +553,24 @@
   </si>
   <si>
     <t xml:space="preserve">Learned of the difficulties in documenting the architecture and social context, and finding interesting issues of software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Mar 2020 (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish homework 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the beginning of this course, I thought, “How can anyone understand a large code base without reading documentation or reading the code senselessly?”. Looking back, I learned a LOT about how to crack the code. These exercises sometimes leave me thinking, “Duh! Why didn’t I think of doing that before?”. The fun is knowing that there is no correct or obvious method to use; it’s a puzzle that only a human and not a computer can solve. Part of the problem is that at the beginning, I understand nothing about the code base. Two months in, and I am getting a feel of how the developers want the code to be. Discovering the code is a work in progress and obviously takes time; it’s like reading between the lines when reading a novel like Lord of the Rings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My head hurts today. Yesterday I had so much energy and today the reverse happens. I long for the verdant lands of Middle Earth as I slowly make my way through the fourth book of Lord of the Rings. I wonder if I still have the Silmarillon lying around somewhere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Mar 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0210</t>
   </si>
 </sst>
 </file>
@@ -746,7 +764,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -789,6 +807,10 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -873,8 +895,8 @@
   </sheetPr>
   <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G48" activeCellId="0" sqref="G48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1673,7 +1695,7 @@
       <c r="D42" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="11" t="s">
         <v>140</v>
       </c>
       <c r="F42" s="8"/>
@@ -1803,20 +1825,41 @@
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
+    <row r="49" customFormat="false" ht="264.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>164</v>
+      </c>
       <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
+      <c r="F49" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
+      <c r="A50" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="8" t="str">
+        <f aca="false">D49</f>
+        <v>Finish homework 5</v>
+      </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>

</xml_diff>

<commit_message>
Updated diary as of 15 Mar 2020
</commit_message>
<xml_diff>
--- a/diaries/diary-harry-duong.xlsx
+++ b/diaries/diary-harry-duong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="189">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -494,6 +494,9 @@
     <t xml:space="preserve">Today I have a monster diet. Android programming (from other courses) takes a lot of energy when doing for the first time.</t>
   </si>
   <si>
+    <t xml:space="preserve">Learned of the difficulties in documenting the architecture and social context, and finding interesting issues of software</t>
+  </si>
+  <si>
     <t xml:space="preserve">27 Feb 2020 (Th)</t>
   </si>
   <si>
@@ -552,7 +555,7 @@
     <t xml:space="preserve">Pull request sent in.</t>
   </si>
   <si>
-    <t xml:space="preserve">Learned of the difficulties in documenting the architecture and social context, and finding interesting issues of software</t>
+    <t xml:space="preserve">Eighth lecture</t>
   </si>
   <si>
     <t xml:space="preserve">4 Mar 2020 (W)</t>
@@ -580,6 +583,54 @@
   </si>
   <si>
     <t xml:space="preserve">With great power comes great responsibility. I enjoy moving back and forth along the working tree in Git; if I mess up, it’s easy to go back. I just can’t wrap my head around the times where Git will merge commits into the same pull request, even though I branch in the correct order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ninth lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Mar 2020 (Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1530-1700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on homework for ninth lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The chaos of the last three weeks, especially with the other two courses from this quarter and the two courses from last quarter are now over. All that remains are the final for this course and the search for the internship. I need to rest badly, lest COVID-19 or another disease take hold of me. Looking back, I had a pleasant time working with Thuc and Deon. Group work was never good throughout many years of schooling and I think this time around, everyone has an incentive to do his/her best. And for that, I must thank Thuc and Deon for changing my opinion on group work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tenth lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Mar 2020 (Sa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1800-1930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More tired than usual. Nutrition and exercise aren’t the issue; something else is wrong. Brain needs rest, and yet I am so used to working actively that I am more comfortable doing something rather than sitting idly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Mar 2020 (Tu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2340-0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feeling better.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Mar 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-1235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Found some interesting test cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most of the test cases in Runelite are surprisingly simple for a large game with a GUI. So it doesn’t seem as scary as I expected.</t>
   </si>
 </sst>
 </file>
@@ -902,10 +953,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1752,81 +1803,81 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="B46" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D46" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E45" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F45" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="F46" s="8" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B46" s="8" t="s">
+      <c r="G46" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="8" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="C47" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="F47" s="8"/>
+      <c r="G47" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C47" s="8" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E47" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>162</v>
@@ -1834,127 +1885,195 @@
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" customFormat="false" ht="264.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" customFormat="false" ht="264.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="8" t="str">
-        <f aca="false">D49</f>
-        <v>Finish homework 5</v>
+      <c r="D50" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-    </row>
-    <row r="51" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F50" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>169</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="8" t="str">
+        <f aca="false">D50</f>
+        <v>Finish homework 5</v>
+      </c>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="C52" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F51" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
+      <c r="F52" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="G52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
+      <c r="A53" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>173</v>
+      </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
+    <row r="54" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>176</v>
+      </c>
       <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
+      <c r="F54" s="8" t="s">
+        <v>177</v>
+      </c>
       <c r="G54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
+      <c r="A55" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>178</v>
+      </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
+    <row r="56" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>176</v>
+      </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
+      <c r="G56" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
+      <c r="A57" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="8" t="str">
+        <f aca="false">D56</f>
+        <v>Work on homework for ninth lecture</v>
+      </c>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
+      <c r="G57" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="8" t="str">
+        <f aca="false">D57</f>
+        <v>Work on homework for ninth lecture</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>188</v>
+      </c>
       <c r="G58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2614,6 +2733,16 @@
       <c r="F131" s="8"/>
       <c r="G131" s="8"/>
     </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="8"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+      <c r="F132" s="8"/>
+      <c r="G132" s="8"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>

</xml_diff>